<commit_message>
added all part no
</commit_message>
<xml_diff>
--- a/doc/Main_BOM.xlsx
+++ b/doc/Main_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soeren\Documents\GitHub\AR2ISS\AR2ISS_MainCTL_HW\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F11D73-7514-44BE-944E-1A0086ECB0C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B73845-B60B-4895-B105-7303397E8869}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23090" yWindow="1890" windowWidth="28800" windowHeight="15460" xr2:uid="{9733E62F-F5BD-478B-A4C8-CFDB1F8BCD57}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="236">
   <si>
     <t xml:space="preserve"> Quantity</t>
   </si>
@@ -712,6 +712,48 @@
   </si>
   <si>
     <t>C14663</t>
+  </si>
+  <si>
+    <t>NTB0102DP-Q100H</t>
+  </si>
+  <si>
+    <t>Not Avaiable</t>
+  </si>
+  <si>
+    <t>700-MAX3232EUET</t>
+  </si>
+  <si>
+    <t>TSR 1-2450E</t>
+  </si>
+  <si>
+    <t>771-PMN48XP115</t>
+  </si>
+  <si>
+    <t>C8598</t>
+  </si>
+  <si>
+    <t>C96230</t>
+  </si>
+  <si>
+    <t>C2128</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>Spalte1</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>523-TSEH09SOL2RM8</t>
+  </si>
+  <si>
+    <t>81-BLM18KG102SN1D</t>
+  </si>
+  <si>
+    <t>511-NUCLEO-H755ZI-Q</t>
   </si>
 </sst>
 </file>
@@ -754,7 +796,10 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -785,29 +830,31 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExterneDaten_1" connectionId="1" xr16:uid="{C0507AAC-8884-4088-9602-A7C0A4C3628D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="7" unboundColumnsRight="1">
-    <queryTableFields count="6">
+  <queryTableRefresh nextId="8" unboundColumnsRight="2">
+    <queryTableFields count="7">
       <queryTableField id="1" name="Reference" tableColumnId="1"/>
       <queryTableField id="2" name=" Quantity" tableColumnId="2"/>
       <queryTableField id="3" name=" Value" tableColumnId="3"/>
       <queryTableField id="4" name=" Footprint" tableColumnId="4"/>
       <queryTableField id="5" name=" Datasheet" tableColumnId="5"/>
       <queryTableField id="6" dataBound="0" tableColumnId="6"/>
+      <queryTableField id="7" dataBound="0" tableColumnId="7"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D58553C-D0E9-42E1-B199-12EE3821C64F}" name="AR2ISS_MainCTL_HW" displayName="AR2ISS_MainCTL_HW" ref="A1:F75" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F75" xr:uid="{874CF72C-6D21-4749-8F6B-49D5CF25BDAE}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{EB4CF8F6-77B1-4EF0-9E22-62F0D16EA59A}" uniqueName="1" name="Designator" queryTableFieldId="1" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D58553C-D0E9-42E1-B199-12EE3821C64F}" name="AR2ISS_MainCTL_HW" displayName="AR2ISS_MainCTL_HW" ref="A1:G75" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G75" xr:uid="{874CF72C-6D21-4749-8F6B-49D5CF25BDAE}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{EB4CF8F6-77B1-4EF0-9E22-62F0D16EA59A}" uniqueName="1" name="Designator" queryTableFieldId="1" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{28965725-DE7B-419F-988C-8269DF2B8493}" uniqueName="2" name=" Quantity" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{89213DB3-B257-4F82-BC99-275E157D9B2A}" uniqueName="3" name=" Value" queryTableFieldId="3" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{80AA46A0-537A-421B-B871-3234F39C9163}" uniqueName="4" name=" Footprint" queryTableFieldId="4" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{1ACDEFEB-711D-44EF-AF1C-1109F9D3A544}" uniqueName="5" name="LCSC Part #" queryTableFieldId="5" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{2F4121E9-C2A9-4027-9A14-3B94401F2B0A}" uniqueName="6" name="Mouser" queryTableFieldId="6" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{89213DB3-B257-4F82-BC99-275E157D9B2A}" uniqueName="3" name=" Value" queryTableFieldId="3" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{80AA46A0-537A-421B-B871-3234F39C9163}" uniqueName="4" name=" Footprint" queryTableFieldId="4" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{1ACDEFEB-711D-44EF-AF1C-1109F9D3A544}" uniqueName="5" name="LCSC Part #" queryTableFieldId="5" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{2F4121E9-C2A9-4027-9A14-3B94401F2B0A}" uniqueName="6" name="Mouser" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{2E6B506E-F79E-4BDB-88C1-B0740DDFE655}" uniqueName="7" name="Spalte1" queryTableFieldId="7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1110,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3BB0A10-05AA-4812-B34D-20EAEE21D6C5}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1124,7 +1171,7 @@
     <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>186</v>
       </c>
@@ -1143,8 +1190,11 @@
       <c r="F1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1159,8 +1209,9 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1175,8 +1226,9 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1192,8 +1244,9 @@
       <c r="E4" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1210,8 +1263,9 @@
         <v>220</v>
       </c>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1228,8 +1282,9 @@
         <v>221</v>
       </c>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1244,8 +1299,9 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1262,8 +1318,9 @@
         <v>19</v>
       </c>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -1278,8 +1335,9 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1296,8 +1354,9 @@
         <v>188</v>
       </c>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -1312,8 +1371,11 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1328,8 +1390,11 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1342,10 +1407,13 @@
       <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
@@ -1358,10 +1426,13 @@
       <c r="D14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1374,10 +1445,13 @@
       <c r="D15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>229</v>
+      </c>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -1394,8 +1468,9 @@
         <v>189</v>
       </c>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1412,8 +1487,9 @@
       <c r="F17" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
@@ -1428,8 +1504,11 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -1444,8 +1523,11 @@
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
@@ -1460,8 +1542,11 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
@@ -1476,8 +1561,11 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
@@ -1492,8 +1580,11 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>60</v>
       </c>
@@ -1508,8 +1599,11 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>63</v>
       </c>
@@ -1524,8 +1618,11 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -1540,8 +1637,11 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
@@ -1556,8 +1656,9 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>70</v>
       </c>
@@ -1572,8 +1673,11 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
@@ -1588,8 +1692,11 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>74</v>
       </c>
@@ -1603,9 +1710,12 @@
         <v>76</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F29" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>77</v>
       </c>
@@ -1620,8 +1730,11 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G30" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>79</v>
       </c>
@@ -1636,8 +1749,9 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>81</v>
       </c>
@@ -1652,8 +1766,11 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G32" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>84</v>
       </c>
@@ -1670,8 +1787,9 @@
         <v>191</v>
       </c>
       <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>87</v>
       </c>
@@ -1685,9 +1803,12 @@
         <v>86</v>
       </c>
       <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F34" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>89</v>
       </c>
@@ -1704,8 +1825,9 @@
         <v>192</v>
       </c>
       <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>91</v>
       </c>
@@ -1722,8 +1844,9 @@
         <v>193</v>
       </c>
       <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>94</v>
       </c>
@@ -1737,9 +1860,12 @@
         <v>96</v>
       </c>
       <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F37" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>97</v>
       </c>
@@ -1754,8 +1880,9 @@
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>100</v>
       </c>
@@ -1772,8 +1899,9 @@
         <v>194</v>
       </c>
       <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>102</v>
       </c>
@@ -1790,8 +1918,9 @@
       <c r="F40" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>105</v>
       </c>
@@ -1808,8 +1937,9 @@
         <v>196</v>
       </c>
       <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>107</v>
       </c>
@@ -1826,8 +1956,9 @@
         <v>197</v>
       </c>
       <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>109</v>
       </c>
@@ -1844,8 +1975,9 @@
         <v>198</v>
       </c>
       <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>111</v>
       </c>
@@ -1862,8 +1994,9 @@
         <v>199</v>
       </c>
       <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>113</v>
       </c>
@@ -1880,8 +2013,9 @@
         <v>200</v>
       </c>
       <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>115</v>
       </c>
@@ -1898,8 +2032,9 @@
         <v>201</v>
       </c>
       <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>117</v>
       </c>
@@ -1916,8 +2051,9 @@
         <v>202</v>
       </c>
       <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>119</v>
       </c>
@@ -1934,8 +2070,9 @@
         <v>203</v>
       </c>
       <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>121</v>
       </c>
@@ -1952,8 +2089,9 @@
         <v>204</v>
       </c>
       <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>123</v>
       </c>
@@ -1970,8 +2108,9 @@
         <v>205</v>
       </c>
       <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>125</v>
       </c>
@@ -1988,8 +2127,9 @@
         <v>206</v>
       </c>
       <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>127</v>
       </c>
@@ -2006,8 +2146,9 @@
         <v>200</v>
       </c>
       <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>129</v>
       </c>
@@ -2024,8 +2165,9 @@
         <v>207</v>
       </c>
       <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>131</v>
       </c>
@@ -2042,8 +2184,9 @@
         <v>201</v>
       </c>
       <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>133</v>
       </c>
@@ -2060,8 +2203,9 @@
         <v>208</v>
       </c>
       <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>135</v>
       </c>
@@ -2078,8 +2222,9 @@
         <v>203</v>
       </c>
       <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>137</v>
       </c>
@@ -2096,8 +2241,9 @@
         <v>209</v>
       </c>
       <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>139</v>
       </c>
@@ -2114,8 +2260,9 @@
         <v>210</v>
       </c>
       <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>141</v>
       </c>
@@ -2132,8 +2279,9 @@
         <v>211</v>
       </c>
       <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>143</v>
       </c>
@@ -2150,8 +2298,9 @@
         <v>212</v>
       </c>
       <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>145</v>
       </c>
@@ -2166,8 +2315,9 @@
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>147</v>
       </c>
@@ -2184,8 +2334,9 @@
         <v>208</v>
       </c>
       <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>149</v>
       </c>
@@ -2202,8 +2353,9 @@
         <v>213</v>
       </c>
       <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>151</v>
       </c>
@@ -2217,9 +2369,12 @@
         <v>153</v>
       </c>
       <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F64" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>154</v>
       </c>
@@ -2233,9 +2388,12 @@
         <v>156</v>
       </c>
       <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F65" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>157</v>
       </c>
@@ -2251,8 +2409,9 @@
       <c r="F66" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>160</v>
       </c>
@@ -2268,8 +2427,9 @@
       <c r="F67" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>163</v>
       </c>
@@ -2286,8 +2446,9 @@
       <c r="F68" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>166</v>
       </c>
@@ -2304,8 +2465,9 @@
       <c r="F69" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>169</v>
       </c>
@@ -2318,10 +2480,13 @@
       <c r="D70" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E70" s="1"/>
+      <c r="E70" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="F70" s="1"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>172</v>
       </c>
@@ -2338,8 +2503,9 @@
         <v>214</v>
       </c>
       <c r="F71" s="1"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>174</v>
       </c>
@@ -2353,9 +2519,12 @@
         <v>168</v>
       </c>
       <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F72" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>176</v>
       </c>
@@ -2372,8 +2541,9 @@
         <v>218</v>
       </c>
       <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>179</v>
       </c>
@@ -2387,9 +2557,12 @@
         <v>181</v>
       </c>
       <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F74" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>182</v>
       </c>
@@ -2406,6 +2579,7 @@
         <v>219</v>
       </c>
       <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>